<commit_message>
2021.04.17 17:48 hoon cli
db스크립트에 단행본 insert 추가
</commit_message>
<xml_diff>
--- a/DB/DB임시파일2.xlsx
+++ b/DB/DB임시파일2.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hoony\Desktop\web\SEMI\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Clientes-hoon\Desktop\development\SEMI3\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3111" uniqueCount="1300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="1305">
   <si>
     <t>회원번호</t>
   </si>
@@ -4953,11 +4953,31 @@
     <t>hllee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>NOV_REVIEW_NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOV_NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REVIEW_DATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOV_CONTENT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7384,15 +7404,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="34.625" bestFit="1" customWidth="1"/>
@@ -7416,195 +7436,213 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1301</v>
       </c>
       <c r="C2" t="s">
-        <v>1283</v>
-      </c>
-      <c r="D2" s="2">
-        <v>43621</v>
+        <v>1302</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1303</v>
       </c>
       <c r="E2" t="s">
-        <v>1284</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="D3" s="2">
-        <v>43624</v>
+        <v>43621</v>
       </c>
       <c r="E3" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="D4" s="2">
-        <v>43626</v>
+        <v>43624</v>
       </c>
       <c r="E4" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="D5" s="2">
-        <v>43628</v>
+        <v>43626</v>
       </c>
       <c r="E5" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>611</v>
+        <v>1289</v>
       </c>
       <c r="D6" s="2">
-        <v>43629</v>
+        <v>43628</v>
       </c>
       <c r="E6" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>1292</v>
+        <v>611</v>
       </c>
       <c r="D7" s="2">
-        <v>43682</v>
+        <v>43629</v>
       </c>
       <c r="E7" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>622</v>
+        <v>1292</v>
       </c>
       <c r="D8" s="2">
-        <v>43686</v>
+        <v>43682</v>
       </c>
       <c r="E8" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>657</v>
+        <v>622</v>
       </c>
       <c r="D9" s="2">
-        <v>43697</v>
+        <v>43686</v>
       </c>
       <c r="E9" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D10" s="2">
-        <v>43723</v>
+        <v>43697</v>
       </c>
       <c r="E10" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>1297</v>
+        <v>662</v>
       </c>
       <c r="D11" s="2">
-        <v>43728</v>
+        <v>43723</v>
       </c>
       <c r="E11" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43728</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>1299</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <v>43733</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>1280</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>